<commit_message>
Finished runs for instrat_hprices2
</commit_message>
<xml_diff>
--- a/outputs/pypsapl_outputs.xlsx
+++ b/outputs/pypsapl_outputs.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,14 +514,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6.51</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>31.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -535,14 +535,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>6.51</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>31.78</v>
       </c>
     </row>
     <row r="6">
@@ -556,14 +556,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>15.34</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>53.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -577,14 +577,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.97</v>
+        <v>15.34</v>
       </c>
       <c r="E7" t="n">
-        <v>2.98</v>
+        <v>53.51</v>
       </c>
     </row>
     <row r="8">
@@ -598,14 +598,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4.73</v>
+        <v>0.97</v>
       </c>
       <c r="E8" t="n">
-        <v>9.15</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="9">
@@ -619,14 +619,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7.88</v>
+        <v>4.73</v>
       </c>
       <c r="E9" t="n">
-        <v>8.539999999999999</v>
+        <v>9.15</v>
       </c>
     </row>
     <row r="10">
@@ -640,14 +640,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>9.82</v>
+        <v>7.88</v>
       </c>
       <c r="E10" t="n">
-        <v>10.77</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -661,14 +661,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>11.03</v>
+        <v>9.82</v>
       </c>
       <c r="E11" t="n">
-        <v>29.39</v>
+        <v>10.77</v>
       </c>
     </row>
     <row r="12">
@@ -682,14 +682,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>11.03</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>29.39</v>
       </c>
     </row>
     <row r="13">
@@ -703,7 +703,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Wind_Off</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -720,18 +720,18 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>Import</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.67</v>
+        <v>5.32</v>
       </c>
       <c r="E14" t="n">
-        <v>5.56</v>
+        <v>25.24</v>
       </c>
     </row>
     <row r="15">
@@ -741,18 +741,18 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Biomass</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1.47</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>10.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -766,14 +766,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Biogas</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>7.93</v>
+        <v>0.67</v>
       </c>
       <c r="E16" t="n">
-        <v>28.75</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="17">
@@ -787,14 +787,14 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Biomass</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1.47</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="18">
@@ -808,14 +808,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>14.27</v>
+        <v>1.2</v>
       </c>
       <c r="E18" t="n">
-        <v>19.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -829,14 +829,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.97</v>
+        <v>7.93</v>
       </c>
       <c r="E19" t="n">
-        <v>2.83</v>
+        <v>28.75</v>
       </c>
     </row>
     <row r="20">
@@ -850,14 +850,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.86</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -871,14 +871,14 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>14.01</v>
+        <v>14.27</v>
       </c>
       <c r="E21" t="n">
-        <v>13.35</v>
+        <v>19.82</v>
       </c>
     </row>
     <row r="22">
@@ -892,14 +892,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>15.01</v>
+        <v>0.97</v>
       </c>
       <c r="E22" t="n">
-        <v>14.72</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="23">
@@ -913,14 +913,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>18.36</v>
+        <v>0.86</v>
       </c>
       <c r="E23" t="n">
-        <v>44.76</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24">
@@ -934,14 +934,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.49</v>
+        <v>14.01</v>
       </c>
       <c r="E24" t="n">
-        <v>32.04</v>
+        <v>13.35</v>
       </c>
     </row>
     <row r="25">
@@ -955,14 +955,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>15.01</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>14.72</v>
       </c>
     </row>
     <row r="26">
@@ -972,18 +972,18 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.92</v>
+        <v>18.36</v>
       </c>
       <c r="E26" t="n">
-        <v>6.59</v>
+        <v>44.76</v>
       </c>
     </row>
     <row r="27">
@@ -993,18 +993,18 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Biomass</t>
+          <t>Wind_Off</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.02</v>
+        <v>7.49</v>
       </c>
       <c r="E27" t="n">
-        <v>5.63</v>
+        <v>32.04</v>
       </c>
     </row>
     <row r="28">
@@ -1014,18 +1014,18 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Import</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>5.78</v>
+        <v>7.32</v>
       </c>
       <c r="E28" t="n">
-        <v>14.03</v>
+        <v>27.54</v>
       </c>
     </row>
     <row r="29">
@@ -1035,11 +1035,11 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1060,14 +1060,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>Biogas</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>10.05</v>
+        <v>0.92</v>
       </c>
       <c r="E30" t="n">
-        <v>12.08</v>
+        <v>6.59</v>
       </c>
     </row>
     <row r="31">
@@ -1081,14 +1081,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Biomass</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.97</v>
+        <v>1.02</v>
       </c>
       <c r="E31" t="n">
-        <v>2.43</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="32">
@@ -1102,14 +1102,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.86</v>
+        <v>1.85</v>
       </c>
       <c r="E32" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1123,14 +1123,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>18.69</v>
+        <v>5.78</v>
       </c>
       <c r="E33" t="n">
-        <v>14.69</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="34">
@@ -1144,14 +1144,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>18.96</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>14.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1165,14 +1165,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>28.23</v>
+        <v>10.05</v>
       </c>
       <c r="E35" t="n">
-        <v>57.51</v>
+        <v>12.08</v>
       </c>
     </row>
     <row r="36">
@@ -1186,14 +1186,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>14.3</v>
+        <v>0.97</v>
       </c>
       <c r="E36" t="n">
-        <v>57.97</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="37">
@@ -1207,14 +1207,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3.95</v>
+        <v>0.86</v>
       </c>
       <c r="E37" t="n">
-        <v>9.09</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="38">
@@ -1224,18 +1224,18 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.17</v>
+        <v>18.69</v>
       </c>
       <c r="E38" t="n">
-        <v>8.74</v>
+        <v>14.69</v>
       </c>
     </row>
     <row r="39">
@@ -1245,18 +1245,18 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Biomass</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.73</v>
+        <v>18.96</v>
       </c>
       <c r="E39" t="n">
-        <v>3.48</v>
+        <v>14.71</v>
       </c>
     </row>
     <row r="40">
@@ -1266,18 +1266,18 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.78</v>
+        <v>28.23</v>
       </c>
       <c r="E40" t="n">
-        <v>14.53</v>
+        <v>57.51</v>
       </c>
     </row>
     <row r="41">
@@ -1287,18 +1287,18 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Wind_Off</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>57.97</v>
       </c>
     </row>
     <row r="42">
@@ -1308,18 +1308,18 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>Import</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7.24</v>
+        <v>8.02</v>
       </c>
       <c r="E42" t="n">
-        <v>11.78</v>
+        <v>17.16</v>
       </c>
     </row>
     <row r="43">
@@ -1329,18 +1329,18 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.97</v>
+        <v>3.95</v>
       </c>
       <c r="E43" t="n">
-        <v>2.49</v>
+        <v>9.09</v>
       </c>
     </row>
     <row r="44">
@@ -1354,14 +1354,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>Biogas</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>1.17</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>8.74</v>
       </c>
     </row>
     <row r="45">
@@ -1375,14 +1375,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Biomass</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>21.91</v>
+        <v>0.73</v>
       </c>
       <c r="E45" t="n">
-        <v>18.89</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="46">
@@ -1396,14 +1396,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>21.69</v>
+        <v>2.5</v>
       </c>
       <c r="E46" t="n">
-        <v>19.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1417,14 +1417,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>36.36</v>
+        <v>5.78</v>
       </c>
       <c r="E47" t="n">
-        <v>80.17</v>
+        <v>14.53</v>
       </c>
     </row>
     <row r="48">
@@ -1438,14 +1438,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>17.88</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>56.45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1459,182 +1459,182 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>5.95</v>
+        <v>7.24</v>
       </c>
       <c r="E49" t="n">
-        <v>12.26</v>
+        <v>11.78</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.42</v>
+        <v>0.97</v>
       </c>
       <c r="E50" t="n">
-        <v>3.67</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Biomass</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1.63</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>12.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6.51</v>
+        <v>21.91</v>
       </c>
       <c r="E52" t="n">
-        <v>13.77</v>
+        <v>18.89</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>21.69</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>19.22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>15.34</v>
+        <v>36.36</v>
       </c>
       <c r="E54" t="n">
-        <v>54.08</v>
+        <v>80.17</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Wind_Off</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.97</v>
+        <v>17.88</v>
       </c>
       <c r="E55" t="n">
-        <v>2.98</v>
+        <v>56.45</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>Import</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>4.73</v>
+        <v>8.02</v>
       </c>
       <c r="E56" t="n">
-        <v>17.05</v>
+        <v>6.18</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>instrat_hprices</t>
+          <t>instrat</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>7.88</v>
+        <v>5.95</v>
       </c>
       <c r="E57" t="n">
-        <v>8.539999999999999</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="58">
@@ -1648,14 +1648,14 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>Biogas</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>9.82</v>
+        <v>0.42</v>
       </c>
       <c r="E58" t="n">
-        <v>10.77</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="59">
@@ -1669,14 +1669,14 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Biomass</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>11.03</v>
+        <v>1.63</v>
       </c>
       <c r="E59" t="n">
-        <v>29.39</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="60">
@@ -1690,11 +1690,11 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -1711,14 +1711,14 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>6.51</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>13.77</v>
       </c>
     </row>
     <row r="62">
@@ -1728,18 +1728,18 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>5.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1749,18 +1749,18 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Biomass</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>1.47</v>
+        <v>15.34</v>
       </c>
       <c r="E63" t="n">
-        <v>10.27</v>
+        <v>54.08</v>
       </c>
     </row>
     <row r="64">
@@ -1770,18 +1770,18 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>7.93</v>
+        <v>0.97</v>
       </c>
       <c r="E64" t="n">
-        <v>16.42</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="65">
@@ -1791,18 +1791,18 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>4.73</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>17.05</v>
       </c>
     </row>
     <row r="66">
@@ -1812,18 +1812,18 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>14.27</v>
+        <v>7.88</v>
       </c>
       <c r="E66" t="n">
-        <v>24.21</v>
+        <v>8.539999999999999</v>
       </c>
     </row>
     <row r="67">
@@ -1833,18 +1833,18 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.97</v>
+        <v>9.82</v>
       </c>
       <c r="E67" t="n">
-        <v>2.86</v>
+        <v>10.77</v>
       </c>
     </row>
     <row r="68">
@@ -1854,18 +1854,18 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.86</v>
+        <v>11.03</v>
       </c>
       <c r="E68" t="n">
-        <v>0.84</v>
+        <v>29.39</v>
       </c>
     </row>
     <row r="69">
@@ -1875,18 +1875,18 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Wind_Off</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>14.01</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>13.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1896,18 +1896,18 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>Import</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>15.01</v>
+        <v>5.32</v>
       </c>
       <c r="E70" t="n">
-        <v>14.82</v>
+        <v>34.78</v>
       </c>
     </row>
     <row r="71">
@@ -1917,18 +1917,18 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Hydrogen</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>18.36</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>44.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1942,14 +1942,14 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>Biogas</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>7.49</v>
+        <v>0.67</v>
       </c>
       <c r="E72" t="n">
-        <v>32.06</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="73">
@@ -1963,14 +1963,14 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Hydrogen</t>
+          <t>Biomass</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>1.47</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="74">
@@ -1980,18 +1980,18 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Biogas</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.92</v>
+        <v>1.2</v>
       </c>
       <c r="E74" t="n">
-        <v>6.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2001,18 +2001,18 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Biomass</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>1.02</v>
+        <v>7.93</v>
       </c>
       <c r="E75" t="n">
-        <v>5.99</v>
+        <v>16.42</v>
       </c>
     </row>
     <row r="76">
@@ -2022,18 +2022,18 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>5.78</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>13.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2043,18 +2043,18 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>14.27</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>24.21</v>
       </c>
     </row>
     <row r="78">
@@ -2064,18 +2064,18 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>10.05</v>
+        <v>0.97</v>
       </c>
       <c r="E78" t="n">
-        <v>12.33</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="79">
@@ -2085,18 +2085,18 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.97</v>
+        <v>0.86</v>
       </c>
       <c r="E79" t="n">
-        <v>2.36</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="80">
@@ -2106,18 +2106,18 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.86</v>
+        <v>14.01</v>
       </c>
       <c r="E80" t="n">
-        <v>0.04</v>
+        <v>13.49</v>
       </c>
     </row>
     <row r="81">
@@ -2127,18 +2127,18 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>18.69</v>
+        <v>15.01</v>
       </c>
       <c r="E81" t="n">
-        <v>14.57</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="82">
@@ -2148,18 +2148,18 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>18.96</v>
+        <v>18.36</v>
       </c>
       <c r="E82" t="n">
-        <v>14.96</v>
+        <v>44.66</v>
       </c>
     </row>
     <row r="83">
@@ -2169,18 +2169,18 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Wind_Off</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>28.23</v>
+        <v>7.49</v>
       </c>
       <c r="E83" t="n">
-        <v>55.12</v>
+        <v>32.06</v>
       </c>
     </row>
     <row r="84">
@@ -2190,18 +2190,18 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>Import</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>14.3</v>
+        <v>7.32</v>
       </c>
       <c r="E84" t="n">
-        <v>60.17</v>
+        <v>34.79</v>
       </c>
     </row>
     <row r="85">
@@ -2211,7 +2211,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2219,10 +2219,10 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>3.95</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>4.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2240,10 +2240,10 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>1.17</v>
+        <v>0.92</v>
       </c>
       <c r="E86" t="n">
-        <v>8.52</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="87">
@@ -2253,7 +2253,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2261,10 +2261,10 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.73</v>
+        <v>1.02</v>
       </c>
       <c r="E87" t="n">
-        <v>3.82</v>
+        <v>5.69</v>
       </c>
     </row>
     <row r="88">
@@ -2274,18 +2274,18 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>DSR</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>5.78</v>
+        <v>1.85</v>
       </c>
       <c r="E88" t="n">
-        <v>14.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2295,18 +2295,18 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Geothermal</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>5.78</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>13.45</v>
       </c>
     </row>
     <row r="90">
@@ -2316,18 +2316,18 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Hard coal</t>
+          <t>Geothermal</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>7.24</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>11.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2337,18 +2337,18 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Hydro</t>
+          <t>Hard coal</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.97</v>
+        <v>10.05</v>
       </c>
       <c r="E91" t="n">
-        <v>2.55</v>
+        <v>12.76</v>
       </c>
     </row>
     <row r="92">
@@ -2358,18 +2358,18 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Lignite</t>
+          <t>Hydro</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>0.97</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="93">
@@ -2379,18 +2379,18 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>PV_Ground</t>
+          <t>Lignite</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>21.91</v>
+        <v>0.86</v>
       </c>
       <c r="E93" t="n">
-        <v>18.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="94">
@@ -2400,18 +2400,18 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>PV_Roof</t>
+          <t>PV_Ground</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>21.69</v>
+        <v>18.69</v>
       </c>
       <c r="E94" t="n">
-        <v>17.88</v>
+        <v>14.41</v>
       </c>
     </row>
     <row r="95">
@@ -2421,18 +2421,18 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>PV_Roof</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>36.36</v>
+        <v>18.96</v>
       </c>
       <c r="E95" t="n">
-        <v>70.95</v>
+        <v>14.97</v>
       </c>
     </row>
     <row r="96">
@@ -2442,18 +2442,18 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Wind_Off</t>
+          <t>Wind</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>17.88</v>
+        <v>28.23</v>
       </c>
       <c r="E96" t="n">
-        <v>65.88</v>
+        <v>56.12</v>
       </c>
     </row>
     <row r="97">
@@ -2463,18 +2463,1530 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
+          <t>Wind_Off</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="E97" t="n">
+        <v>59.07</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>8.02</v>
+      </c>
+      <c r="E98" t="n">
+        <v>21.89</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
           <t>Hydrogen</t>
         </is>
       </c>
-      <c r="D97" t="n">
+      <c r="D99" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="E99" t="n">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E100" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Biomass</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E101" t="n">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>DSR</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E103" t="n">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Geothermal</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Hard coal</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>7.24</v>
+      </c>
+      <c r="E105" t="n">
+        <v>11.27</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Hydro</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E106" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Lignite</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>PV_Ground</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>21.91</v>
+      </c>
+      <c r="E108" t="n">
+        <v>18.27</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>PV_Roof</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="E109" t="n">
+        <v>18.42</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="E110" t="n">
+        <v>75.93000000000001</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Wind_Off</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>17.88</v>
+      </c>
+      <c r="E111" t="n">
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>8.02</v>
+      </c>
+      <c r="E112" t="n">
+        <v>15.21</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>instrat_hprices</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
         <v>5.95</v>
       </c>
-      <c r="E97" t="n">
+      <c r="E113" t="n">
         <v>3.23</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="E114" t="n">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Biomass</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="E115" t="n">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>DSR</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>6.51</v>
+      </c>
+      <c r="E117" t="n">
+        <v>13.76</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Geothermal</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Hard coal</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>15.34</v>
+      </c>
+      <c r="E119" t="n">
+        <v>72.87</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Hydro</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E120" t="n">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Lignite</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="E121" t="n">
+        <v>32.36</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>PV_Ground</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>7.88</v>
+      </c>
+      <c r="E122" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>PV_Roof</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="E123" t="n">
+        <v>10.77</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>11.03</v>
+      </c>
+      <c r="E124" t="n">
+        <v>29.4</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Wind_Off</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="E126" t="n">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="E128" t="n">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Biomass</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="E129" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>DSR</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>7.93</v>
+      </c>
+      <c r="E131" t="n">
+        <v>18.74</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Geothermal</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Hard coal</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>14.27</v>
+      </c>
+      <c r="E133" t="n">
+        <v>52.05</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Hydro</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E134" t="n">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Lignite</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="E135" t="n">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>PV_Ground</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>14.01</v>
+      </c>
+      <c r="E136" t="n">
+        <v>13.54</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>PV_Roof</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>15.01</v>
+      </c>
+      <c r="E137" t="n">
+        <v>14.51</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>18.36</v>
+      </c>
+      <c r="E138" t="n">
+        <v>45.43</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Wind_Off</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="E139" t="n">
+        <v>32.01</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="E140" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E142" t="n">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Biomass</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="E143" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>DSR</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E145" t="n">
+        <v>13.94</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Geothermal</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>0</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Hard coal</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>10.05</v>
+      </c>
+      <c r="E147" t="n">
+        <v>20.35</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Hydro</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E148" t="n">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Lignite</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="E149" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>PV_Ground</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>18.69</v>
+      </c>
+      <c r="E150" t="n">
+        <v>14.57</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>PV_Roof</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>18.96</v>
+      </c>
+      <c r="E151" t="n">
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>28.23</v>
+      </c>
+      <c r="E152" t="n">
+        <v>55.22</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Wind_Off</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="E153" t="n">
+        <v>59.79</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>8.02</v>
+      </c>
+      <c r="E154" t="n">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="E155" t="n">
+        <v>13.39</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E156" t="n">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Biomass</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E157" t="n">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>DSR</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E159" t="n">
+        <v>13.77</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Geothermal</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>0</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Hard coal</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>7.24</v>
+      </c>
+      <c r="E161" t="n">
+        <v>11.36</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Hydro</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E162" t="n">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Lignite</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>0</v>
+      </c>
+      <c r="E163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>PV_Ground</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>21.91</v>
+      </c>
+      <c r="E164" t="n">
+        <v>17.86</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>PV_Roof</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="E165" t="n">
+        <v>17.26</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Wind</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="E166" t="n">
+        <v>74.25</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Wind_Off</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>17.88</v>
+      </c>
+      <c r="E167" t="n">
+        <v>64.33</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>8.02</v>
+      </c>
+      <c r="E168" t="n">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Hydrogen</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="E169" t="n">
+        <v>13.62</v>
       </c>
     </row>
   </sheetData>
@@ -2488,7 +4000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2617,6 +4129,58 @@
         <v>158.56</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C10" t="n">
+        <v>507.77</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2030</v>
+      </c>
+      <c r="C11" t="n">
+        <v>449.92</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2035</v>
+      </c>
+      <c r="C12" t="n">
+        <v>303.19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>instrat_hprices2</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2040</v>
+      </c>
+      <c r="C13" t="n">
+        <v>252.38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>